<commit_message>
finish notice of course
</commit_message>
<xml_diff>
--- a/code/backend/online-edu/src/test/resources/UserData.xlsx
+++ b/code/backend/online-edu/src/test/resources/UserData.xlsx
@@ -40,7 +40,7 @@
     <t>grade</t>
   </si>
   <si>
-    <t>real name</t>
+    <t>realname</t>
   </si>
   <si>
     <t>sex</t>
@@ -802,9 +802,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -823,8 +823,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -838,15 +884,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -854,30 +894,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -891,17 +915,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -920,51 +966,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -975,7 +976,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -987,7 +994,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -999,67 +1084,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1077,55 +1120,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1137,25 +1138,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1194,30 +1195,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1247,11 +1224,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1269,145 +1270,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1416,7 +1417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="48" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1736,10 +1737,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J201"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1887,7 +1888,7 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D5">
@@ -1983,7 +1984,7 @@
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8">
@@ -4408,445 +4409,90 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="3:3">
-      <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="3:3">
-      <c r="C85" s="2"/>
-    </row>
-    <row r="86" spans="3:3">
-      <c r="C86" s="2"/>
-    </row>
-    <row r="87" spans="3:3">
-      <c r="C87" s="2"/>
-    </row>
-    <row r="88" spans="3:3">
-      <c r="C88" s="2"/>
-    </row>
-    <row r="89" spans="3:3">
-      <c r="C89" s="2"/>
-    </row>
-    <row r="90" spans="3:3">
-      <c r="C90" s="2"/>
-    </row>
-    <row r="91" spans="3:3">
-      <c r="C91" s="2"/>
-    </row>
-    <row r="92" spans="3:3">
-      <c r="C92" s="2"/>
-    </row>
-    <row r="93" spans="3:3">
-      <c r="C93" s="2"/>
-    </row>
-    <row r="94" spans="3:3">
-      <c r="C94" s="2"/>
-    </row>
-    <row r="95" spans="3:3">
-      <c r="C95" s="2"/>
-    </row>
-    <row r="96" spans="3:3">
-      <c r="C96" s="2"/>
-    </row>
-    <row r="97" spans="3:3">
-      <c r="C97" s="2"/>
-    </row>
-    <row r="98" spans="3:3">
-      <c r="C98" s="2"/>
-    </row>
-    <row r="99" spans="3:3">
-      <c r="C99" s="2"/>
-    </row>
-    <row r="100" spans="3:3">
-      <c r="C100" s="2"/>
-    </row>
-    <row r="101" spans="3:3">
-      <c r="C101" s="2"/>
-    </row>
-    <row r="102" spans="3:3">
-      <c r="C102" s="3"/>
-    </row>
-    <row r="103" spans="3:3">
-      <c r="C103" s="3"/>
-    </row>
-    <row r="104" spans="3:3">
-      <c r="C104" s="3"/>
-    </row>
-    <row r="105" spans="3:3">
-      <c r="C105" s="3"/>
-    </row>
-    <row r="106" spans="3:3">
-      <c r="C106" s="3"/>
-    </row>
-    <row r="107" spans="3:3">
-      <c r="C107" s="3"/>
-    </row>
-    <row r="108" spans="3:3">
-      <c r="C108" s="3"/>
-    </row>
-    <row r="109" spans="3:3">
-      <c r="C109" s="3"/>
-    </row>
-    <row r="110" spans="3:3">
-      <c r="C110" s="3"/>
-    </row>
-    <row r="111" spans="3:3">
-      <c r="C111" s="3"/>
-    </row>
-    <row r="112" spans="3:3">
-      <c r="C112" s="3"/>
-    </row>
-    <row r="113" spans="3:3">
-      <c r="C113" s="3"/>
-    </row>
-    <row r="114" spans="3:3">
-      <c r="C114" s="3"/>
-    </row>
-    <row r="115" spans="3:3">
-      <c r="C115" s="3"/>
-    </row>
-    <row r="116" spans="3:3">
-      <c r="C116" s="3"/>
-    </row>
-    <row r="117" spans="3:3">
-      <c r="C117" s="3"/>
-    </row>
-    <row r="118" spans="3:3">
-      <c r="C118" s="3"/>
-    </row>
-    <row r="119" spans="3:3">
-      <c r="C119" s="3"/>
-    </row>
-    <row r="120" spans="3:3">
-      <c r="C120" s="3"/>
-    </row>
-    <row r="121" spans="3:3">
-      <c r="C121" s="3"/>
-    </row>
-    <row r="122" spans="3:3">
-      <c r="C122" s="3"/>
-    </row>
-    <row r="123" spans="3:3">
-      <c r="C123" s="3"/>
-    </row>
-    <row r="124" spans="3:3">
-      <c r="C124" s="3"/>
-    </row>
-    <row r="125" spans="3:3">
-      <c r="C125" s="3"/>
-    </row>
-    <row r="126" spans="3:3">
-      <c r="C126" s="3"/>
-    </row>
-    <row r="127" spans="3:3">
-      <c r="C127" s="3"/>
-    </row>
-    <row r="128" spans="3:3">
-      <c r="C128" s="3"/>
-    </row>
-    <row r="129" spans="3:3">
-      <c r="C129" s="3"/>
-    </row>
-    <row r="130" spans="3:3">
-      <c r="C130" s="3"/>
-    </row>
-    <row r="131" spans="3:3">
-      <c r="C131" s="3"/>
-    </row>
-    <row r="132" spans="3:3">
-      <c r="C132" s="3"/>
-    </row>
-    <row r="133" spans="3:3">
-      <c r="C133" s="3"/>
-    </row>
-    <row r="134" spans="3:3">
-      <c r="C134" s="3"/>
-    </row>
-    <row r="135" spans="3:3">
-      <c r="C135" s="3"/>
-    </row>
-    <row r="136" spans="3:3">
-      <c r="C136" s="3"/>
-    </row>
-    <row r="137" spans="3:3">
-      <c r="C137" s="3"/>
-    </row>
-    <row r="138" spans="3:3">
-      <c r="C138" s="3"/>
-    </row>
-    <row r="139" spans="3:3">
-      <c r="C139" s="3"/>
-    </row>
-    <row r="140" spans="3:3">
-      <c r="C140" s="3"/>
-    </row>
-    <row r="141" spans="3:3">
-      <c r="C141" s="3"/>
-    </row>
-    <row r="142" spans="3:3">
-      <c r="C142" s="3"/>
-    </row>
-    <row r="143" spans="3:3">
-      <c r="C143" s="3"/>
-    </row>
-    <row r="144" spans="3:3">
-      <c r="C144" s="3"/>
-    </row>
-    <row r="145" spans="3:3">
-      <c r="C145" s="3"/>
-    </row>
-    <row r="146" spans="3:3">
-      <c r="C146" s="3"/>
-    </row>
-    <row r="147" spans="3:3">
-      <c r="C147" s="3"/>
-    </row>
-    <row r="148" spans="3:3">
-      <c r="C148" s="3"/>
-    </row>
-    <row r="149" spans="3:3">
-      <c r="C149" s="3"/>
-    </row>
-    <row r="150" spans="3:3">
-      <c r="C150" s="3"/>
-    </row>
-    <row r="151" spans="3:3">
-      <c r="C151" s="3"/>
-    </row>
-    <row r="152" spans="3:3">
-      <c r="C152" s="3"/>
-    </row>
-    <row r="153" spans="3:3">
-      <c r="C153" s="3"/>
-    </row>
-    <row r="154" spans="3:3">
-      <c r="C154" s="3"/>
-    </row>
-    <row r="155" spans="3:3">
-      <c r="C155" s="3"/>
-    </row>
-    <row r="156" spans="3:3">
-      <c r="C156" s="3"/>
-    </row>
-    <row r="157" spans="3:3">
-      <c r="C157" s="3"/>
-    </row>
-    <row r="158" spans="3:3">
-      <c r="C158" s="3"/>
-    </row>
-    <row r="159" spans="3:3">
-      <c r="C159" s="3"/>
-    </row>
-    <row r="160" spans="3:3">
-      <c r="C160" s="3"/>
-    </row>
-    <row r="161" spans="3:3">
-      <c r="C161" s="3"/>
-    </row>
-    <row r="162" spans="3:3">
-      <c r="C162" s="3"/>
-    </row>
-    <row r="163" spans="3:3">
-      <c r="C163" s="3"/>
-    </row>
-    <row r="164" spans="3:3">
-      <c r="C164" s="3"/>
-    </row>
-    <row r="165" spans="3:3">
-      <c r="C165" s="3"/>
-    </row>
-    <row r="166" spans="3:3">
-      <c r="C166" s="3"/>
-    </row>
-    <row r="167" spans="3:3">
-      <c r="C167" s="3"/>
-    </row>
-    <row r="168" spans="3:3">
-      <c r="C168" s="3"/>
-    </row>
-    <row r="169" spans="3:3">
-      <c r="C169" s="3"/>
-    </row>
-    <row r="170" spans="3:3">
-      <c r="C170" s="3"/>
-    </row>
-    <row r="171" spans="3:3">
-      <c r="C171" s="3"/>
-    </row>
-    <row r="172" spans="3:3">
-      <c r="C172" s="3"/>
-    </row>
-    <row r="173" spans="3:3">
-      <c r="C173" s="3"/>
-    </row>
-    <row r="174" spans="3:3">
-      <c r="C174" s="3"/>
-    </row>
-    <row r="175" spans="3:3">
-      <c r="C175" s="3"/>
-    </row>
-    <row r="176" spans="3:3">
-      <c r="C176" s="3"/>
-    </row>
-    <row r="177" spans="3:3">
-      <c r="C177" s="3"/>
-    </row>
-    <row r="178" spans="3:3">
-      <c r="C178" s="3"/>
-    </row>
-    <row r="179" spans="3:3">
-      <c r="C179" s="3"/>
-    </row>
-    <row r="180" spans="3:3">
-      <c r="C180" s="3"/>
-    </row>
-    <row r="181" spans="3:3">
-      <c r="C181" s="3"/>
-    </row>
-    <row r="182" spans="3:3">
-      <c r="C182" s="3"/>
-    </row>
-    <row r="183" spans="3:3">
-      <c r="C183" s="3"/>
-    </row>
-    <row r="184" spans="3:3">
-      <c r="C184" s="3"/>
-    </row>
-    <row r="185" spans="3:3">
-      <c r="C185" s="3"/>
-    </row>
-    <row r="186" spans="3:3">
-      <c r="C186" s="3"/>
-    </row>
-    <row r="187" spans="3:3">
-      <c r="C187" s="3"/>
-    </row>
-    <row r="188" spans="3:3">
-      <c r="C188" s="3"/>
-    </row>
-    <row r="189" spans="3:3">
-      <c r="C189" s="3"/>
-    </row>
-    <row r="190" spans="3:3">
-      <c r="C190" s="3"/>
-    </row>
-    <row r="191" spans="3:3">
-      <c r="C191" s="3"/>
-    </row>
-    <row r="192" spans="3:3">
-      <c r="C192" s="3"/>
-    </row>
-    <row r="193" spans="3:3">
-      <c r="C193" s="3"/>
-    </row>
-    <row r="194" spans="3:3">
-      <c r="C194" s="3"/>
-    </row>
-    <row r="195" spans="3:3">
-      <c r="C195" s="3"/>
-    </row>
-    <row r="196" spans="3:3">
-      <c r="C196" s="3"/>
-    </row>
-    <row r="197" spans="3:3">
-      <c r="C197" s="3"/>
-    </row>
-    <row r="198" spans="3:3">
-      <c r="C198" s="3"/>
-    </row>
-    <row r="199" spans="3:3">
-      <c r="C199" s="3"/>
-    </row>
-    <row r="200" spans="3:3">
-      <c r="C200" s="3"/>
-    </row>
-    <row r="201" spans="3:3">
-      <c r="C201" s="3"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C103:C201" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2" display="students1@qq.com"/>
-    <hyperlink ref="C3" r:id="rId3" display="students2@qq.com"/>
-    <hyperlink ref="C4" r:id="rId2" display="students3@qq.com"/>
-    <hyperlink ref="C6" r:id="rId2" display="students5@qq.com"/>
-    <hyperlink ref="C8" r:id="rId2" display="students7@qq.com"/>
-    <hyperlink ref="C10" r:id="rId2" display="students9@qq.com"/>
-    <hyperlink ref="C12" r:id="rId2" display="students11@qq.com"/>
-    <hyperlink ref="C14" r:id="rId2" display="students13@qq.com"/>
-    <hyperlink ref="C16" r:id="rId2" display="students15@qq.com"/>
-    <hyperlink ref="C18" r:id="rId2" display="students17@qq.com"/>
-    <hyperlink ref="C20" r:id="rId2" display="students19@qq.com"/>
-    <hyperlink ref="C22" r:id="rId2" display="students21@qq.com"/>
-    <hyperlink ref="C24" r:id="rId2" display="students23@qq.com"/>
-    <hyperlink ref="C26" r:id="rId2" display="students25@qq.com"/>
-    <hyperlink ref="C28" r:id="rId2" display="students27@qq.com"/>
-    <hyperlink ref="C30" r:id="rId2" display="students29@qq.com"/>
-    <hyperlink ref="C32" r:id="rId2" display="students31@qq.com"/>
-    <hyperlink ref="C34" r:id="rId2" display="students33@qq.com"/>
-    <hyperlink ref="C36" r:id="rId2" display="students35@qq.com"/>
-    <hyperlink ref="C38" r:id="rId2" display="students37@qq.com"/>
-    <hyperlink ref="C40" r:id="rId2" display="students39@qq.com"/>
-    <hyperlink ref="C42" r:id="rId2" display="students41@qq.com"/>
-    <hyperlink ref="C44" r:id="rId2" display="students43@qq.com"/>
-    <hyperlink ref="C46" r:id="rId2" display="students45@qq.com"/>
-    <hyperlink ref="C48" r:id="rId2" display="students47@qq.com"/>
-    <hyperlink ref="C50" r:id="rId2" display="students49@qq.com"/>
-    <hyperlink ref="C52" r:id="rId2" display="students51@qq.com"/>
-    <hyperlink ref="C54" r:id="rId2" display="students53@qq.com"/>
-    <hyperlink ref="C56" r:id="rId2" display="students55@qq.com"/>
-    <hyperlink ref="C58" r:id="rId2" display="students57@qq.com"/>
-    <hyperlink ref="C60" r:id="rId2" display="students59@qq.com"/>
-    <hyperlink ref="C62" r:id="rId2" display="students61@qq.com"/>
-    <hyperlink ref="C64" r:id="rId2" display="students63@qq.com"/>
-    <hyperlink ref="C66" r:id="rId2" display="students65@qq.com"/>
-    <hyperlink ref="C68" r:id="rId2" display="students67@qq.com"/>
-    <hyperlink ref="C70" r:id="rId2" display="students69@qq.com"/>
-    <hyperlink ref="C72" r:id="rId2" display="students71@qq.com"/>
-    <hyperlink ref="C74" r:id="rId2" display="students73@qq.com"/>
-    <hyperlink ref="C76" r:id="rId2" display="students75@qq.com"/>
-    <hyperlink ref="C78" r:id="rId2" display="students77@qq.com"/>
-    <hyperlink ref="C80" r:id="rId2" display="students79@qq.com"/>
-    <hyperlink ref="C82" r:id="rId2" display="students81@qq.com"/>
-    <hyperlink ref="C5" r:id="rId3" display="students4@qq.com"/>
-    <hyperlink ref="C7" r:id="rId3" display="students6@qq.com"/>
-    <hyperlink ref="C9" r:id="rId3" display="students8@qq.com"/>
-    <hyperlink ref="C11" r:id="rId3" display="students10@qq.com"/>
-    <hyperlink ref="C13" r:id="rId3" display="students12@qq.com"/>
-    <hyperlink ref="C15" r:id="rId3" display="students14@qq.com"/>
-    <hyperlink ref="C17" r:id="rId3" display="students16@qq.com"/>
-    <hyperlink ref="C19" r:id="rId3" display="students18@qq.com"/>
-    <hyperlink ref="C21" r:id="rId3" display="students20@qq.com"/>
-    <hyperlink ref="C23" r:id="rId3" display="students22@qq.com"/>
-    <hyperlink ref="C25" r:id="rId3" display="students24@qq.com"/>
-    <hyperlink ref="C27" r:id="rId3" display="students26@qq.com"/>
-    <hyperlink ref="C29" r:id="rId3" display="students28@qq.com"/>
-    <hyperlink ref="C31" r:id="rId3" display="students30@qq.com"/>
-    <hyperlink ref="C33" r:id="rId3" display="students32@qq.com"/>
-    <hyperlink ref="C35" r:id="rId3" display="students34@qq.com"/>
-    <hyperlink ref="C37" r:id="rId3" display="students36@qq.com"/>
-    <hyperlink ref="C39" r:id="rId3" display="students38@qq.com"/>
-    <hyperlink ref="C41" r:id="rId3" display="students40@qq.com"/>
-    <hyperlink ref="C43" r:id="rId3" display="students42@qq.com"/>
-    <hyperlink ref="C45" r:id="rId3" display="students44@qq.com"/>
-    <hyperlink ref="C47" r:id="rId3" display="students46@qq.com"/>
-    <hyperlink ref="C49" r:id="rId3" display="students48@qq.com"/>
-    <hyperlink ref="C51" r:id="rId3" display="students50@qq.com"/>
-    <hyperlink ref="C53" r:id="rId3" display="students52@qq.com"/>
-    <hyperlink ref="C55" r:id="rId3" display="students54@qq.com"/>
-    <hyperlink ref="C57" r:id="rId3" display="students56@qq.com"/>
-    <hyperlink ref="C59" r:id="rId3" display="students58@qq.com"/>
-    <hyperlink ref="C61" r:id="rId3" display="students60@qq.com"/>
-    <hyperlink ref="C63" r:id="rId3" display="students62@qq.com"/>
-    <hyperlink ref="C65" r:id="rId3" display="students64@qq.com"/>
-    <hyperlink ref="C67" r:id="rId3" display="students66@qq.com"/>
-    <hyperlink ref="C69" r:id="rId3" display="students68@qq.com"/>
-    <hyperlink ref="C71" r:id="rId3" display="students70@qq.com"/>
-    <hyperlink ref="C73" r:id="rId3" display="students72@qq.com"/>
-    <hyperlink ref="C75" r:id="rId3" display="students74@qq.com"/>
-    <hyperlink ref="C77" r:id="rId3" display="students76@qq.com"/>
-    <hyperlink ref="C79" r:id="rId3" display="students78@qq.com"/>
-    <hyperlink ref="C81" r:id="rId3" display="students80@qq.com"/>
-    <hyperlink ref="C83" r:id="rId3" display="students82@qq.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="students1@qq.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="students2@qq.com"/>
+    <hyperlink ref="C4" r:id="rId1" display="students3@qq.com"/>
+    <hyperlink ref="C6" r:id="rId1" display="students5@qq.com"/>
+    <hyperlink ref="C8" r:id="rId1" display="students7@qq.com"/>
+    <hyperlink ref="C10" r:id="rId1" display="students9@qq.com"/>
+    <hyperlink ref="C12" r:id="rId1" display="students11@qq.com"/>
+    <hyperlink ref="C14" r:id="rId1" display="students13@qq.com"/>
+    <hyperlink ref="C16" r:id="rId1" display="students15@qq.com"/>
+    <hyperlink ref="C18" r:id="rId1" display="students17@qq.com"/>
+    <hyperlink ref="C20" r:id="rId1" display="students19@qq.com"/>
+    <hyperlink ref="C22" r:id="rId1" display="students21@qq.com"/>
+    <hyperlink ref="C24" r:id="rId1" display="students23@qq.com"/>
+    <hyperlink ref="C26" r:id="rId1" display="students25@qq.com"/>
+    <hyperlink ref="C28" r:id="rId1" display="students27@qq.com"/>
+    <hyperlink ref="C30" r:id="rId1" display="students29@qq.com"/>
+    <hyperlink ref="C32" r:id="rId1" display="students31@qq.com"/>
+    <hyperlink ref="C34" r:id="rId1" display="students33@qq.com"/>
+    <hyperlink ref="C36" r:id="rId1" display="students35@qq.com"/>
+    <hyperlink ref="C38" r:id="rId1" display="students37@qq.com"/>
+    <hyperlink ref="C40" r:id="rId1" display="students39@qq.com"/>
+    <hyperlink ref="C42" r:id="rId1" display="students41@qq.com"/>
+    <hyperlink ref="C44" r:id="rId1" display="students43@qq.com"/>
+    <hyperlink ref="C46" r:id="rId1" display="students45@qq.com"/>
+    <hyperlink ref="C48" r:id="rId1" display="students47@qq.com"/>
+    <hyperlink ref="C50" r:id="rId1" display="students49@qq.com"/>
+    <hyperlink ref="C52" r:id="rId1" display="students51@qq.com"/>
+    <hyperlink ref="C54" r:id="rId1" display="students53@qq.com"/>
+    <hyperlink ref="C56" r:id="rId1" display="students55@qq.com"/>
+    <hyperlink ref="C58" r:id="rId1" display="students57@qq.com"/>
+    <hyperlink ref="C60" r:id="rId1" display="students59@qq.com"/>
+    <hyperlink ref="C62" r:id="rId1" display="students61@qq.com"/>
+    <hyperlink ref="C64" r:id="rId1" display="students63@qq.com"/>
+    <hyperlink ref="C66" r:id="rId1" display="students65@qq.com"/>
+    <hyperlink ref="C68" r:id="rId1" display="students67@qq.com"/>
+    <hyperlink ref="C70" r:id="rId1" display="students69@qq.com"/>
+    <hyperlink ref="C72" r:id="rId1" display="students71@qq.com"/>
+    <hyperlink ref="C74" r:id="rId1" display="students73@qq.com"/>
+    <hyperlink ref="C76" r:id="rId1" display="students75@qq.com"/>
+    <hyperlink ref="C78" r:id="rId1" display="students77@qq.com"/>
+    <hyperlink ref="C80" r:id="rId1" display="students79@qq.com"/>
+    <hyperlink ref="C82" r:id="rId1" display="students81@qq.com"/>
+    <hyperlink ref="C5" r:id="rId2" display="students4@qq.com"/>
+    <hyperlink ref="C7" r:id="rId2" display="students6@qq.com"/>
+    <hyperlink ref="C9" r:id="rId2" display="students8@qq.com"/>
+    <hyperlink ref="C11" r:id="rId2" display="students10@qq.com"/>
+    <hyperlink ref="C13" r:id="rId2" display="students12@qq.com"/>
+    <hyperlink ref="C15" r:id="rId2" display="students14@qq.com"/>
+    <hyperlink ref="C17" r:id="rId2" display="students16@qq.com"/>
+    <hyperlink ref="C19" r:id="rId2" display="students18@qq.com"/>
+    <hyperlink ref="C21" r:id="rId2" display="students20@qq.com"/>
+    <hyperlink ref="C23" r:id="rId2" display="students22@qq.com"/>
+    <hyperlink ref="C25" r:id="rId2" display="students24@qq.com"/>
+    <hyperlink ref="C27" r:id="rId2" display="students26@qq.com"/>
+    <hyperlink ref="C29" r:id="rId2" display="students28@qq.com"/>
+    <hyperlink ref="C31" r:id="rId2" display="students30@qq.com"/>
+    <hyperlink ref="C33" r:id="rId2" display="students32@qq.com"/>
+    <hyperlink ref="C35" r:id="rId2" display="students34@qq.com"/>
+    <hyperlink ref="C37" r:id="rId2" display="students36@qq.com"/>
+    <hyperlink ref="C39" r:id="rId2" display="students38@qq.com"/>
+    <hyperlink ref="C41" r:id="rId2" display="students40@qq.com"/>
+    <hyperlink ref="C43" r:id="rId2" display="students42@qq.com"/>
+    <hyperlink ref="C45" r:id="rId2" display="students44@qq.com"/>
+    <hyperlink ref="C47" r:id="rId2" display="students46@qq.com"/>
+    <hyperlink ref="C49" r:id="rId2" display="students48@qq.com"/>
+    <hyperlink ref="C51" r:id="rId2" display="students50@qq.com"/>
+    <hyperlink ref="C53" r:id="rId2" display="students52@qq.com"/>
+    <hyperlink ref="C55" r:id="rId2" display="students54@qq.com"/>
+    <hyperlink ref="C57" r:id="rId2" display="students56@qq.com"/>
+    <hyperlink ref="C59" r:id="rId2" display="students58@qq.com"/>
+    <hyperlink ref="C61" r:id="rId2" display="students60@qq.com"/>
+    <hyperlink ref="C63" r:id="rId2" display="students62@qq.com"/>
+    <hyperlink ref="C65" r:id="rId2" display="students64@qq.com"/>
+    <hyperlink ref="C67" r:id="rId2" display="students66@qq.com"/>
+    <hyperlink ref="C69" r:id="rId2" display="students68@qq.com"/>
+    <hyperlink ref="C71" r:id="rId2" display="students70@qq.com"/>
+    <hyperlink ref="C73" r:id="rId2" display="students72@qq.com"/>
+    <hyperlink ref="C75" r:id="rId2" display="students74@qq.com"/>
+    <hyperlink ref="C77" r:id="rId2" display="students76@qq.com"/>
+    <hyperlink ref="C79" r:id="rId2" display="students78@qq.com"/>
+    <hyperlink ref="C81" r:id="rId2" display="students80@qq.com"/>
+    <hyperlink ref="C83" r:id="rId2" display="students82@qq.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>